<commit_message>
update import and account
</commit_message>
<xml_diff>
--- a/SEP490_G67/MyAPI/wwwroot/templates/Template_Trip_Convenience.xlsx
+++ b/SEP490_G67/MyAPI/wwwroot/templates/Template_Trip_Convenience.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="TripConvenience" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Trip to Phố Nỉ</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Phố Nỉ</t>
-  </si>
-  <si>
-    <t>98B-01273</t>
   </si>
   <si>
     <r>
@@ -151,7 +148,29 @@
     </r>
   </si>
   <si>
-    <t>* Lưu ý: Tất cả các trường đánh dấu * đều phải điền đầy đủ thông tin.  Làm đúng theo yêu cầu.</t>
+    <t>30A-09120</t>
+  </si>
+  <si>
+    <t>30A-09121</t>
+  </si>
+  <si>
+    <t>30A-30952</t>
+  </si>
+  <si>
+    <t>Loại chuyến đi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+* Lưu ý: Tất cả các trường đánh dấu * đều phải điền đầy đủ thông tin.  Làm đúng theo yêu cầu.</t>
+  </si>
+  <si>
+    <t>Giá trị</t>
+  </si>
+  <si>
+    <t>Tiện chuyến</t>
+  </si>
+  <si>
+    <t>Bao xe</t>
   </si>
 </sst>
 </file>
@@ -213,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -236,20 +255,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -260,24 +270,19 @@
     <xf numFmtId="21" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,55 +563,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -617,45 +625,109 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
         <v>40000</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>40000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J5" s="8">
+        <v>2</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J6" s="8">
+        <v>3</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I2:M3"/>
+    <mergeCell ref="J2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>